<commit_message>
test plan/procedure for daniel created, fixed nelian's
</commit_message>
<xml_diff>
--- a/Test Plans - HH2/test_procedure_Nelian.xlsx
+++ b/Test Plans - HH2/test_procedure_Nelian.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelian\Downloads\skydrive-2013-10-22 (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelian\Documents\GitHub\Capstone\Test Plans - HH2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152510"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="124">
   <si>
     <t>Reviewed by:</t>
   </si>
@@ -238,15 +237,9 @@
     <t>Node.js</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
-    <t>To run all the tests go to home/panda and run sudo npm test</t>
-  </si>
-  <si>
     <t>Run the same instructions for create project (existent project)</t>
   </si>
   <si>
@@ -256,9 +249,6 @@
     <t>res.statusCode must be 404</t>
   </si>
   <si>
-    <t>Create a gitlab instance. Create a project with desired user_id (2) and desired project name (happyhour) (params = {user_id: 2, name: 'happyhour'}. Call gitlab.project.create(params, callback)</t>
-  </si>
-  <si>
     <t>res.statusCode must be 200</t>
   </si>
   <si>
@@ -392,6 +382,15 @@
   </si>
   <si>
     <t>Text editor (Sublime Text)</t>
+  </si>
+  <si>
+    <t>To run all the tests go to home/panda and run sudo npm test. For all tests beginning with G, an instance of gitlab is required. For the tests beginning with S, an instance of sendgrid is required.</t>
+  </si>
+  <si>
+    <t>Create a project with desired user_id (2) and desired project name (happyhour) (params = {user_id: 2, name: 'happyhour'}  by calling gitlab.project.create(params, callback)</t>
+  </si>
+  <si>
+    <t>Mongo DB</t>
   </si>
 </sst>
 </file>
@@ -612,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -628,21 +627,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -653,11 +637,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -665,29 +670,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -970,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,42 +989,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="14">
         <v>41584</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="13"/>
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -1032,583 +1034,608 @@
       <c r="B6" s="12"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="25"/>
+      <c r="D7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="D8" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="24"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="16">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="D8" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="25"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="28" t="s">
+      <c r="D18" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="29" t="s">
+      <c r="D19" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="16">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="29" t="s">
+      <c r="E21" s="16">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D22" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="29" t="s">
+      <c r="E22" s="16">
+        <v>1</v>
+      </c>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="29" t="s">
+      <c r="D23" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>72</v>
+      <c r="E23" s="16">
+        <v>1</v>
       </c>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="16">
+        <v>1</v>
+      </c>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C25" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="16">
+        <v>1</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="16">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="7"/>
+      <c r="D27" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="16">
+        <v>1</v>
+      </c>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="16">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C29" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="16">
+        <v>1</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" s="16">
+        <v>1</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="29" t="s">
+      <c r="E31" s="16">
+        <v>1</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="29" t="s">
+      <c r="D32" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="16">
+        <v>1</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D30" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="8"/>
+      <c r="D33" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="16">
+        <v>1</v>
+      </c>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="16">
+        <v>1</v>
+      </c>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C35" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="16">
+        <v>1</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D36" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="16">
+        <v>1</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="29" t="s">
+      <c r="D37" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="16">
+        <v>1</v>
+      </c>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E38" s="16">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="29" t="s">
+      <c r="D39" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="29" t="s">
+      <c r="E39" s="16">
+        <v>1</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="29" t="s">
+      <c r="D40" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="E40" s="16">
+        <v>1</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E38" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="29" t="s">
+      <c r="D41" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="E41" s="16">
+        <v>1</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E39" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="29" t="s">
+      <c r="D42" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" s="16">
+        <v>1</v>
+      </c>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D43" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" s="20"/>
+      <c r="E43" s="34">
+        <v>1</v>
+      </c>
+      <c r="F43" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A7:B7"/>
+  <mergeCells count="10">
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E13"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
+  <conditionalFormatting sqref="E17:E42">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to test procedure and gantt chart
</commit_message>
<xml_diff>
--- a/Test Plans - HH2/test_procedure_Nelian.xlsx
+++ b/Test Plans - HH2/test_procedure_Nelian.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="146">
   <si>
     <t>Reviewed by:</t>
   </si>
@@ -683,45 +683,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -749,6 +710,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -756,6 +756,235 @@
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -794,235 +1023,6 @@
         </horizontal>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1037,16 +1037,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A17:G48" totalsRowShown="0" headerRowDxfId="0" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="A17:G48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A17:G44" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A17:G44"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Test ID" dataDxfId="7"/>
-    <tableColumn id="2" name="Test Description" dataDxfId="6"/>
-    <tableColumn id="3" name="Instructions" dataDxfId="5"/>
-    <tableColumn id="4" name="Parameters" dataDxfId="4"/>
-    <tableColumn id="5" name="Expected Outcome" dataDxfId="3"/>
-    <tableColumn id="6" name="Pass/Fail" dataDxfId="2"/>
-    <tableColumn id="7" name="Comments" dataDxfId="1"/>
+    <tableColumn id="1" name="Test ID" dataDxfId="6"/>
+    <tableColumn id="2" name="Test Description" dataDxfId="5"/>
+    <tableColumn id="3" name="Instructions" dataDxfId="4"/>
+    <tableColumn id="4" name="Parameters" dataDxfId="3"/>
+    <tableColumn id="5" name="Expected Outcome" dataDxfId="2"/>
+    <tableColumn id="6" name="Pass/Fail" dataDxfId="1"/>
+    <tableColumn id="7" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1315,9 +1315,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
@@ -1325,10 +1328,11 @@
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1379,104 +1383,104 @@
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="E7" s="9" t="s">
+      <c r="B7" s="33"/>
+      <c r="E7" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="E8" s="11" t="s">
+      <c r="B8" s="30"/>
+      <c r="E8" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="B9" s="30"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
+      <c r="B10" s="30"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
+      <c r="B11" s="30"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
+      <c r="B12" s="30"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="16"/>
+      <c r="B13" s="30"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="B14" s="30"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="20"/>
+      <c r="B15" s="32"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1494,12 +1498,12 @@
       <c r="F18" s="8">
         <v>1</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="18" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1517,10 +1521,10 @@
       <c r="F19" s="8">
         <v>1</v>
       </c>
-      <c r="G19" s="32"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="10" t="s">
         <v>44</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1529,17 +1533,19 @@
       <c r="C20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="E20" s="7" t="s">
         <v>89</v>
       </c>
       <c r="F20" s="8">
         <v>1</v>
       </c>
-      <c r="G20" s="32"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1557,10 +1563,10 @@
       <c r="F21" s="8">
         <v>1</v>
       </c>
-      <c r="G21" s="32"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1578,12 +1584,12 @@
       <c r="F22" s="8">
         <v>1</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="19" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1601,10 +1607,10 @@
       <c r="F23" s="8">
         <v>1</v>
       </c>
-      <c r="G23" s="32"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -1622,12 +1628,12 @@
       <c r="F24" s="8">
         <v>1</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="18" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="10" t="s">
         <v>49</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -1645,10 +1651,10 @@
       <c r="F25" s="8">
         <v>1</v>
       </c>
-      <c r="G25" s="32"/>
+      <c r="G25" s="19"/>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1666,157 +1672,169 @@
       <c r="F26" s="8">
         <v>1</v>
       </c>
-      <c r="G26" s="24"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="24"/>
-    </row>
-    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
+      <c r="B27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="8">
+        <v>1</v>
+      </c>
+      <c r="G27" s="19"/>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="B28" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F28" s="8">
         <v>1</v>
       </c>
-      <c r="G28" s="32"/>
+      <c r="G28" s="19"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>52</v>
+      <c r="A29" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F29" s="8">
         <v>1</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>53</v>
+      <c r="A30" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>128</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F30" s="8">
         <v>1</v>
       </c>
-      <c r="G30" s="24"/>
+      <c r="G30" s="11" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>54</v>
+      <c r="A31" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F31" s="8">
         <v>1</v>
       </c>
-      <c r="G31" s="24" t="s">
-        <v>131</v>
-      </c>
+      <c r="G31" s="11"/>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>55</v>
+      <c r="A32" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F32" s="8">
         <v>1</v>
       </c>
-      <c r="G32" s="24"/>
+      <c r="G32" s="11"/>
     </row>
     <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
-        <v>56</v>
+      <c r="A33" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>135</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F33" s="8">
         <v>1</v>
       </c>
-      <c r="G33" s="24"/>
+      <c r="G33" s="11"/>
     </row>
     <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>57</v>
+      <c r="A34" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>89</v>
@@ -1824,269 +1842,221 @@
       <c r="F34" s="8">
         <v>1</v>
       </c>
-      <c r="G34" s="24"/>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>58</v>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F35" s="8">
         <v>1</v>
       </c>
-      <c r="G35" s="24"/>
+      <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>59</v>
+      <c r="A36" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F36" s="8">
         <v>1</v>
       </c>
-      <c r="G36" s="24"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="24"/>
-    </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>60</v>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="8">
+        <v>1</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F38" s="8">
         <v>1</v>
       </c>
-      <c r="G38" s="24"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="24"/>
-    </row>
-    <row r="40" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
-        <v>61</v>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" s="8">
+        <v>1</v>
+      </c>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="F40" s="8">
         <v>1</v>
       </c>
-      <c r="G40" s="33" t="s">
-        <v>102</v>
+      <c r="G40" s="20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
-        <v>62</v>
+      <c r="A41" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E41" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" s="8">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="8">
+        <v>1</v>
+      </c>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F41" s="8">
-        <v>1</v>
-      </c>
-      <c r="G41" s="24"/>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F42" s="8">
-        <v>1</v>
-      </c>
-      <c r="G42" s="24"/>
-    </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="F43" s="8">
         <v>1</v>
       </c>
-      <c r="G43" s="33" t="s">
-        <v>103</v>
-      </c>
+      <c r="G43" s="11"/>
     </row>
     <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F44" s="8">
-        <v>1</v>
-      </c>
-      <c r="G44" s="24"/>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F45" s="8">
-        <v>1</v>
-      </c>
-      <c r="G45" s="24"/>
-    </row>
-    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F46" s="8">
-        <v>1</v>
-      </c>
-      <c r="G46" s="24"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="24"/>
-    </row>
-    <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A44" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="25" t="s">
+      <c r="C44" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D44" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E44" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="F48" s="26">
-        <v>1</v>
-      </c>
-      <c r="G48" s="27"/>
+      <c r="F44" s="13">
+        <v>1</v>
+      </c>
+      <c r="G44" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -2102,16 +2072,7 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
   </mergeCells>
-  <conditionalFormatting sqref="F18:F47">
-    <cfRule type="iconSet" priority="2">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F48">
+  <conditionalFormatting sqref="F44">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2120,8 +2081,17 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <conditionalFormatting sqref="F18:F43">
+    <cfRule type="iconSet" priority="6">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
+  <pageSetup scale="77" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>